<commit_message>
Extend repository-import excel with new dossier-manager role.
</commit_message>
<xml_diff>
--- a/opengever/setup/tests/assets/testcontentx.xlsx
+++ b/opengever/setup/tests/assets/testcontentx.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1040" windowWidth="46180" windowHeight="21480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,13 +12,13 @@
   <definedNames>
     <definedName name="repository" localSheetId="0">Sheet1!$A$6:$X$47</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Registraturplan Appenzell I.Rh.</t>
   </si>
@@ -240,6 +235,12 @@
   </si>
   <si>
     <t>Default Row</t>
+  </si>
+  <si>
+    <t>manage_dossiers_access</t>
+  </si>
+  <si>
+    <t>Dossier Verwalten</t>
   </si>
 </sst>
 </file>
@@ -249,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -292,6 +293,20 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -359,29 +374,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -417,9 +418,31 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -474,7 +497,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -509,7 +532,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -686,7 +709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -696,13 +719,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
     <col min="3" max="3" width="40.33203125" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
@@ -729,128 +752,130 @@
     <col min="26" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="13">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="3"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="E2" s="14"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2"/>
+    <row r="2" spans="1:23" s="4" customFormat="1" ht="7" customHeight="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="E2" s="8"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="1" t="s">
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="W3"/>
+      <c r="W3" s="14" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" s="10" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="97" customHeight="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="18" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
     </row>
-    <row r="5" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="20" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -914,8 +939,11 @@
       <c r="V5" t="s">
         <v>44</v>
       </c>
+      <c r="W5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -940,13 +968,13 @@
       <c r="M6">
         <v>30</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="13">
         <v>40452</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="13">
         <v>47786</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="P6" s="13" t="s">
         <v>50</v>
       </c>
       <c r="R6" t="s">
@@ -965,8 +993,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:23">
+      <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B7" t="s">
@@ -993,12 +1021,15 @@
       <c r="M7">
         <v>30</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="13">
         <v>40452</v>
       </c>
+      <c r="W7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:23">
+      <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B8" t="s">
@@ -1022,7 +1053,7 @@
       <c r="M8">
         <v>20</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="13">
         <v>40452</v>
       </c>
       <c r="Q8">
@@ -1044,7 +1075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -1053,7 +1084,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="L3:L4"/>
@@ -1061,18 +1103,13 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle translations for block_inheritance in repository xlsx file.
</commit_message>
<xml_diff>
--- a/opengever/setup/tests/assets/testcontentx.xlsx
+++ b/opengever/setup/tests/assets/testcontentx.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Work/development/opengever.core/opengever/setup/tests/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC7DA33B-0C5A-6848-8847-074C2E1A8AF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="repository" localSheetId="0">Sheet1!$A$6:$X$47</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Registraturplan Appenzell I.Rh.</t>
   </si>
@@ -225,9 +234,6 @@
     <t>Nicht öffentlich</t>
   </si>
   <si>
-    <t>Archivwürdig</t>
-  </si>
-  <si>
     <t>GROUP_C</t>
   </si>
   <si>
@@ -241,16 +247,25 @@
   </si>
   <si>
     <t>Dossier Verwalten</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>archival worthy</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -310,7 +325,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +338,14 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -373,6 +394,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -381,7 +417,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -418,31 +454,33 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -450,8 +488,26 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Ordnungssystem"/>
+      <sheetName val="Wertebereich"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -709,21 +765,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
@@ -752,7 +808,7 @@
     <col min="26" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="13">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -791,51 +847,51 @@
       <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="V3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="14" t="s">
-        <v>70</v>
+      <c r="W3" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="4" customFormat="1" ht="97" customHeight="1">
@@ -848,14 +904,14 @@
         <v>19</v>
       </c>
       <c r="E4" s="19"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="12" t="s">
         <v>20</v>
       </c>
@@ -868,12 +924,12 @@
       <c r="Q4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
     </row>
     <row r="5" spans="1:23" ht="20" customHeight="1">
       <c r="A5" t="s">
@@ -940,7 +996,7 @@
         <v>44</v>
       </c>
       <c r="W5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -977,6 +1033,9 @@
       <c r="P6" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="Q6" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="R6" t="s">
         <v>51</v>
       </c>
@@ -1024,6 +1083,9 @@
       <c r="N7" s="13">
         <v>40452</v>
       </c>
+      <c r="Q7" t="s">
+        <v>70</v>
+      </c>
       <c r="W7" t="s">
         <v>51</v>
       </c>
@@ -1047,8 +1109,8 @@
       <c r="I8">
         <v>20</v>
       </c>
-      <c r="K8" t="s">
-        <v>65</v>
+      <c r="K8" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="M8">
         <v>20</v>
@@ -1060,31 +1122,35 @@
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -1099,14 +1165,26 @@
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6E1B58F-9916-1C4A-976C-6BFE10945E0E}">
+          <x14:formula1>
+            <xm:f>'/Work/development/opengever.core/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/[ordnungssystem.xlsx]Wertebereich'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1F0DC928-8CE5-D346-B56F-23B82E9F30FD}">
+          <x14:formula1>
+            <xm:f>'/Work/development/opengever.core/opengever/examplecontent/profiles/repository_minimal/opengever_repositories/[ordnungssystem.xlsx]Wertebereich'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
Remove IRestrictedDossier behavior and addable_dossier_types field
</commit_message>
<xml_diff>
--- a/opengever/setup/tests/assets/testcontentx.xlsx
+++ b/opengever/setup/tests/assets/testcontentx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Work/development/opengever.core/opengever/setup/tests/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinagerber/Documents/ftw_packages/opengever.core/opengever/setup/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC7DA33B-0C5A-6848-8847-074C2E1A8AF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E516E6F2-A425-A841-BE90-15F8C5D98B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="repository" localSheetId="0">Sheet1!$A$6:$X$47</definedName>
+    <definedName name="repository" localSheetId="0">Sheet1!$A$6:$W$47</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Registraturplan Appenzell I.Rh.</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Gültig bis</t>
   </si>
   <si>
-    <t>Addable dossier types</t>
-  </si>
-  <si>
     <t>Unterbruch Vererbung</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>valid_until</t>
   </si>
   <si>
-    <t>addable_dossier_types</t>
-  </si>
-  <si>
     <t>block_inheritance</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
   </si>
   <si>
     <t>Nicht geprüft</t>
-  </si>
-  <si>
-    <t>opengever.dossier.special1, opengever.dossier.special2</t>
   </si>
   <si>
     <t>GROUP_A</t>
@@ -265,7 +256,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -455,6 +446,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -470,17 +465,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -773,13 +764,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
@@ -796,19 +787,18 @@
     <col min="13" max="13" width="13.83203125" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="18" max="18" width="7.83203125" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" customWidth="1"/>
-    <col min="21" max="21" width="18.83203125" customWidth="1"/>
-    <col min="22" max="23" width="18.1640625" customWidth="1"/>
-    <col min="24" max="24" width="19.1640625" customWidth="1"/>
-    <col min="25" max="25" width="23.1640625" customWidth="1"/>
-    <col min="26" max="1025" width="11" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="7.83203125" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="19" max="19" width="15.83203125" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" customWidth="1"/>
+    <col min="21" max="22" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" customWidth="1"/>
+    <col min="24" max="24" width="23.1640625" customWidth="1"/>
+    <col min="25" max="1024" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="14">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -816,102 +806,101 @@
       <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" ht="7" customHeight="1">
+    <row r="2" spans="1:22" s="4" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="E2" s="8"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:22" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="15" t="s">
+      <c r="P3" s="10"/>
+      <c r="Q3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="R3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="S3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="T3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="U3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="15" t="s">
-        <v>69</v>
+      <c r="V3" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="97" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
+    <row r="4" spans="1:22" s="4" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="12" t="s">
         <v>20</v>
       </c>
@@ -921,105 +910,99 @@
       <c r="P4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+    </row>
+    <row r="5" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" ht="20" customHeight="1">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T5" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="V5" t="s">
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="W5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M6">
         <v>30</v>
@@ -1030,52 +1013,49 @@
       <c r="O6" s="13">
         <v>47786</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="P6" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="S6" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="T6" t="s">
-        <v>52</v>
-      </c>
-      <c r="U6" t="s">
-        <v>52</v>
-      </c>
-      <c r="V6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="1" t="s">
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
         <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
       </c>
       <c r="I7">
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M7">
         <v>30</v>
@@ -1083,34 +1063,34 @@
       <c r="N7" s="13">
         <v>40452</v>
       </c>
-      <c r="Q7" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7" t="s">
-        <v>51</v>
+      <c r="P7" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H8" t="s">
         <v>61</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>64</v>
       </c>
       <c r="I8">
         <v>20</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M8">
         <v>20</v>
@@ -1118,53 +1098,53 @@
       <c r="N8" s="13">
         <v>40452</v>
       </c>
-      <c r="Q8">
+      <c r="P8">
         <v>1</v>
       </c>
+      <c r="Q8" t="s">
+        <v>62</v>
+      </c>
       <c r="R8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U8" t="s">
-        <v>65</v>
-      </c>
-      <c r="V8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="T3:T4"/>
     <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>